<commit_message>
Actualización archivo de pesos y dimensiones
</commit_message>
<xml_diff>
--- a/Pesos y dimensiones.xlsx
+++ b/Pesos y dimensiones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Archivos MAAJI\E-commerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923644E-D18B-44B4-BBA1-C9236EB55A08}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F74E969-38FF-463C-9956-AE4DB73192D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{47236B28-B93D-4164-900D-7E069283A063}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="1" activeTab="5" xr2:uid="{47236B28-B93D-4164-900D-7E069283A063}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;D Bottoms Swim" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="164">
   <si>
     <t>SAC - XS</t>
   </si>
@@ -318,6 +318,210 @@
   </si>
   <si>
     <t>COSMETIQUERAS Y SOBRES</t>
+  </si>
+  <si>
+    <t>1930sbc01</t>
+  </si>
+  <si>
+    <t>1930sbc02</t>
+  </si>
+  <si>
+    <t>1932sbc02</t>
+  </si>
+  <si>
+    <t>1943sbc01</t>
+  </si>
+  <si>
+    <t>1943sbc03</t>
+  </si>
+  <si>
+    <t>1943sbc04</t>
+  </si>
+  <si>
+    <t>2023sbc01</t>
+  </si>
+  <si>
+    <t>2024sbc04</t>
+  </si>
+  <si>
+    <t>2024sbc05</t>
+  </si>
+  <si>
+    <t>2024sbc06</t>
+  </si>
+  <si>
+    <t>2041sbc01</t>
+  </si>
+  <si>
+    <t>2041sbc02</t>
+  </si>
+  <si>
+    <t>2041sbc03</t>
+  </si>
+  <si>
+    <t>2041sbc05</t>
+  </si>
+  <si>
+    <t>2041sbc07</t>
+  </si>
+  <si>
+    <t>2041sbc08</t>
+  </si>
+  <si>
+    <t>2043sbc01</t>
+  </si>
+  <si>
+    <t>2043sbc02</t>
+  </si>
+  <si>
+    <t>2043sbc03</t>
+  </si>
+  <si>
+    <t>2043sbc05</t>
+  </si>
+  <si>
+    <t>2043sbc07</t>
+  </si>
+  <si>
+    <t>2043sbc08</t>
+  </si>
+  <si>
+    <t>2043sbc09</t>
+  </si>
+  <si>
+    <t>2047sbc02</t>
+  </si>
+  <si>
+    <t>2047sbc04</t>
+  </si>
+  <si>
+    <t>2047sbc05</t>
+  </si>
+  <si>
+    <t>2050sbc01</t>
+  </si>
+  <si>
+    <t>2061sbc02</t>
+  </si>
+  <si>
+    <t>2061sbc03</t>
+  </si>
+  <si>
+    <t>2061sbc04</t>
+  </si>
+  <si>
+    <t>2061sbc05</t>
+  </si>
+  <si>
+    <t>2062sbc02</t>
+  </si>
+  <si>
+    <t>2062sbc03</t>
+  </si>
+  <si>
+    <t>2062sbc04</t>
+  </si>
+  <si>
+    <t>2062sbc06</t>
+  </si>
+  <si>
+    <t>2062sbc07</t>
+  </si>
+  <si>
+    <t>2062sbc09</t>
+  </si>
+  <si>
+    <t>2062sbc10</t>
+  </si>
+  <si>
+    <t>2062sbc11</t>
+  </si>
+  <si>
+    <t>2062sbc12</t>
+  </si>
+  <si>
+    <t>2062sbc13</t>
+  </si>
+  <si>
+    <t>166 gramos</t>
+  </si>
+  <si>
+    <t>79 gramos</t>
+  </si>
+  <si>
+    <t>61 gramos</t>
+  </si>
+  <si>
+    <t>160 gramos</t>
+  </si>
+  <si>
+    <t>331 gramos</t>
+  </si>
+  <si>
+    <t>90 Gramos</t>
+  </si>
+  <si>
+    <t>Vestidos --&gt; 190 G</t>
+  </si>
+  <si>
+    <t>Camiseta --&gt; 160 G</t>
+  </si>
+  <si>
+    <t>Shorts --&gt; 145 G</t>
+  </si>
+  <si>
+    <t>Busos --&gt; 350 G</t>
+  </si>
+  <si>
+    <t>Leggings --&gt; 154 G</t>
+  </si>
+  <si>
+    <t>Tops</t>
+  </si>
+  <si>
+    <t>Pareos --&gt; 118 G</t>
+  </si>
+  <si>
+    <t>Faldas --&gt; 200 G</t>
+  </si>
+  <si>
+    <t>Shorts --&gt; 165 G</t>
+  </si>
+  <si>
+    <t>Top --&gt; 80 G</t>
+  </si>
+  <si>
+    <t>Pantalones --&gt; 290 G</t>
+  </si>
+  <si>
+    <t>241 Gramos</t>
+  </si>
+  <si>
+    <t>Pequeño --&gt;  26 Gramos</t>
+  </si>
+  <si>
+    <t>Grande --&gt; 360</t>
+  </si>
+  <si>
+    <t>Pequeño --&gt;  160</t>
+  </si>
+  <si>
+    <t>Mediano --&gt; 269 G</t>
+  </si>
+  <si>
+    <t>35 Gramos --&gt; balaca</t>
+  </si>
+  <si>
+    <t>77 Gramos --&gt; visera</t>
+  </si>
+  <si>
+    <t>40 Gramos</t>
+  </si>
+  <si>
+    <t>7 Gramos --&gt; Chulos</t>
+  </si>
+  <si>
+    <t>Niñas --&gt;100 Gramos</t>
   </si>
 </sst>
 </file>
@@ -673,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B107176-5D42-458C-B66D-1CE1BED89986}">
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,170 +965,315 @@
       <c r="A4" t="s">
         <v>44</v>
       </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
+      <c r="G6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
+      <c r="G9" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
+      <c r="G10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
+      <c r="G11" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
+      <c r="G13" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
+      <c r="G15" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
+      </c>
+      <c r="G37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -934,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D999A7A-2212-412D-ABAF-D1B3E4EFD3F5}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,6 +1361,44 @@
         <v>38</v>
       </c>
     </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K3" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" t="s">
+        <v>141</v>
+      </c>
+      <c r="M3" t="s">
+        <v>141</v>
+      </c>
+      <c r="N3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O3" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>141</v>
+      </c>
+      <c r="R3" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" t="s">
+        <v>141</v>
+      </c>
+      <c r="T3" t="s">
+        <v>141</v>
+      </c>
+      <c r="U3" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1019,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3866220-3B84-46DE-85FE-C197893CBF44}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,6 +1476,57 @@
         <v>43</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1096,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D34720-AF5B-49E5-954E-3A37A3134E75}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,6 +1561,20 @@
         <v>43</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1130,9 +1582,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1A672A-E924-4C7B-BDDC-B16E8F5BB5DB}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1183,6 +1637,14 @@
       </c>
       <c r="M2" s="2" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1196,15 +1658,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5EB1C-E591-4408-8281-ABC6014B6115}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1227,6 +1691,39 @@
         <v>95</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>